<commit_message>
refactor: Refactor ZZZDataExe.py for improved readability and maintainability
</commit_message>
<xml_diff>
--- a/doc/绝区零下载UID.xlsx
+++ b/doc/绝区零下载UID.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9180" firstSheet="1" activeTab="3"/>
+    <workbookView windowWidth="27945" windowHeight="12255" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="下载" sheetId="1" r:id="rId1"/>
@@ -14939,6 +14939,9 @@
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
                 </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -15075,6 +15078,9 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="42">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -15300,6 +15306,9 @@
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
                 </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -15430,7 +15439,10 @@
                   <c:v>339.7745003</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>373.1898976</c:v>
+                  <c:v>392.4398953</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>385.5791327</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15655,6 +15667,9 @@
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
                 </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -15785,7 +15800,10 @@
                   <c:v>71.3598897312198</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>48.5221059736753</c:v>
+                  <c:v>52.6219249781913</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>68.2166539522328</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16010,6 +16028,9 @@
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
                 </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -16137,7 +16158,10 @@
                   <c:v>54.3349414197105</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>41.1028237147036</c:v>
+                  <c:v>42.9566734515848</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>35.9687811748137</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16362,6 +16386,9 @@
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
                 </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -16486,7 +16513,10 @@
                   <c:v>40.9323225361819</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>34.2770840364495</c:v>
+                  <c:v>35.899505670253</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>36.8990082741623</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16711,6 +16741,9 @@
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
                 </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -16832,7 +16865,10 @@
                   <c:v>45.6413507925568</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>32.9416132298346</c:v>
+                  <c:v>34.9790055248619</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>26.6665101813274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17056,6 +17092,9 @@
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
                 </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -17174,7 +17213,10 @@
                   <c:v>35.4988283942109</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>30.7158285521431</c:v>
+                  <c:v>32.6777551613841</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>37.0540461240538</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17399,6 +17441,9 @@
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
                 </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -17517,7 +17562,10 @@
                   <c:v>38.7589248793935</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>35.9093261334233</c:v>
+                  <c:v>38.3541727246293</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>30.6974942785048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17739,6 +17787,9 @@
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
                 </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -17851,7 +17902,10 @@
                   <c:v>2001.69924190214</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1919.66509168635</c:v>
+                  <c:v>2008.07106717069</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2020.9183733349</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18202,10 +18256,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>日活跃2!$B$2:$B$44</c:f>
+              <c:f>日活跃2!$B$2:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45477</c:v>
                 </c:pt>
@@ -18334,16 +18388,19 @@
                 </c:pt>
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
+                </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>日活跃2!$C$2:$C$44</c:f>
+              <c:f>日活跃2!$C$2:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>0_ </c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
                   <c:v>1550</c:v>
                 </c:pt>
@@ -18468,7 +18525,10 @@
                   <c:v>264.409598479448</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>298.133971291866</c:v>
+                  <c:v>303.840039741679</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>297.719087635054</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18505,10 +18565,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>日活跃2!$B$2:$B$44</c:f>
+              <c:f>日活跃2!$B$2:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45477</c:v>
                 </c:pt>
@@ -18637,16 +18697,19 @@
                 </c:pt>
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
+                </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>日活跃2!$D$2:$D$44</c:f>
+              <c:f>日活跃2!$D$2:$D$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="1" c:formatCode="0_ ">
                   <c:v>170</c:v>
                 </c:pt>
@@ -18730,10 +18793,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>日活跃2!$B$2:$B$44</c:f>
+              <c:f>日活跃2!$B$2:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45477</c:v>
                 </c:pt>
@@ -18862,16 +18925,19 @@
                 </c:pt>
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
+                </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>日活跃2!$E$2:$E$44</c:f>
+              <c:f>日活跃2!$E$2:$E$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="2" c:formatCode="0_ ">
                   <c:v>100</c:v>
                 </c:pt>
@@ -18952,10 +19018,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>日活跃2!$B$2:$B$44</c:f>
+              <c:f>日活跃2!$B$2:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45477</c:v>
                 </c:pt>
@@ -19084,16 +19150,19 @@
                 </c:pt>
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
+                </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>日活跃2!$F$2:$F$44</c:f>
+              <c:f>日活跃2!$F$2:$F$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="3" c:formatCode="0_ ">
                   <c:v>110</c:v>
                 </c:pt>
@@ -19171,10 +19240,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>日活跃2!$B$2:$B$44</c:f>
+              <c:f>日活跃2!$B$2:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45477</c:v>
                 </c:pt>
@@ -19303,16 +19372,19 @@
                 </c:pt>
                 <c:pt idx="42" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45519</c:v>
+                </c:pt>
+                <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45520</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>日活跃2!$G$2:$G$44</c:f>
+              <c:f>日活跃2!$G$2:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="43"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="4" c:formatCode="0_ ">
                   <c:v>60</c:v>
                 </c:pt>
@@ -29147,8 +29219,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8836660" y="473710"/>
-        <a:ext cx="11172190" cy="5626100"/>
+        <a:off x="9762490" y="450850"/>
+        <a:ext cx="12436475" cy="5271770"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -29177,8 +29249,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8806180" y="589280"/>
-        <a:ext cx="11431905" cy="5311140"/>
+        <a:off x="9732010" y="554990"/>
+        <a:ext cx="12696190" cy="4979670"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -29207,8 +29279,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8811260" y="6186170"/>
-        <a:ext cx="11172190" cy="5626100"/>
+        <a:off x="9737090" y="5808980"/>
+        <a:ext cx="12436475" cy="5271770"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -29242,8 +29314,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3373120" y="20403820"/>
-        <a:ext cx="12246610" cy="6044565"/>
+        <a:off x="3729990" y="19135090"/>
+        <a:ext cx="13565505" cy="5667375"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -29277,8 +29349,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="23703915" y="275590"/>
-        <a:ext cx="8799830" cy="5819140"/>
+        <a:off x="26319480" y="260350"/>
+        <a:ext cx="9759950" cy="5321935"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -29312,8 +29384,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6589395" y="133350"/>
-        <a:ext cx="8778875" cy="5020945"/>
+        <a:off x="7298690" y="133350"/>
+        <a:ext cx="9730105" cy="4700905"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -29347,8 +29419,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6337935" y="117475"/>
-        <a:ext cx="6707505" cy="5530850"/>
+        <a:off x="6979920" y="117475"/>
+        <a:ext cx="7485380" cy="5187950"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -29382,8 +29454,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8887460" y="170180"/>
-        <a:ext cx="5092065" cy="6658610"/>
+        <a:off x="9860280" y="170180"/>
+        <a:ext cx="5621655" cy="6235700"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -29417,8 +29489,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6602095" y="109220"/>
-        <a:ext cx="8985885" cy="5188585"/>
+        <a:off x="7328535" y="109220"/>
+        <a:ext cx="9937115" cy="4862830"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -29447,8 +29519,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6851015" y="5410200"/>
-        <a:ext cx="8985885" cy="5188585"/>
+        <a:off x="7577455" y="5078730"/>
+        <a:ext cx="10005060" cy="4865370"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -30131,7 +30203,7 @@
       <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="7.66666666666667" customWidth="1"/>
     <col min="2" max="2" width="6.66666666666667" style="15" customWidth="1"/>
@@ -30142,9 +30214,9 @@
     <col min="9" max="9" width="3.66666666666667" customWidth="1"/>
     <col min="10" max="12" width="8.66666666666667" customWidth="1"/>
     <col min="13" max="13" width="6.66666666666667" style="12" customWidth="1"/>
-    <col min="14" max="14" width="15.2222222222222" customWidth="1"/>
-    <col min="15" max="15" width="17.5555555555556" customWidth="1"/>
-    <col min="17" max="17" width="12.8888888888889"/>
+    <col min="14" max="14" width="15.225" customWidth="1"/>
+    <col min="15" max="15" width="17.5583333333333" customWidth="1"/>
+    <col min="17" max="17" width="12.8916666666667"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:15">
@@ -34557,26 +34629,26 @@
       <selection activeCell="F162" sqref="F161:F162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="16.4444444444444" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.4416666666667" style="13" customWidth="1"/>
     <col min="2" max="2" width="6.66666666666667" customWidth="1"/>
     <col min="3" max="3" width="9.66666666666667" customWidth="1"/>
-    <col min="4" max="4" width="14.1111111111111" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.4444444444444" customWidth="1"/>
+    <col min="4" max="4" width="14.1083333333333" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.4416666666667" customWidth="1"/>
     <col min="6" max="6" width="6.66666666666667" customWidth="1"/>
-    <col min="7" max="7" width="11.7777777777778" customWidth="1"/>
+    <col min="7" max="7" width="11.775" customWidth="1"/>
     <col min="8" max="8" width="8.66666666666667" customWidth="1"/>
-    <col min="9" max="9" width="16.4444444444444" customWidth="1"/>
+    <col min="9" max="9" width="16.4416666666667" customWidth="1"/>
     <col min="10" max="10" width="6.66666666666667" customWidth="1"/>
-    <col min="11" max="11" width="11.7777777777778" customWidth="1"/>
+    <col min="11" max="11" width="11.775" customWidth="1"/>
     <col min="12" max="12" width="8.66666666666667" customWidth="1"/>
-    <col min="13" max="13" width="17.5555555555556"/>
-    <col min="14" max="14" width="12.8888888888889"/>
-    <col min="15" max="15" width="11.7777777777778" customWidth="1"/>
-    <col min="17" max="17" width="16.4444444444444" customWidth="1"/>
+    <col min="13" max="13" width="17.5583333333333"/>
+    <col min="14" max="14" width="12.8916666666667"/>
+    <col min="15" max="15" width="11.775" customWidth="1"/>
+    <col min="17" max="17" width="16.4416666666667" customWidth="1"/>
     <col min="18" max="18" width="6.66666666666667" customWidth="1"/>
-    <col min="19" max="19" width="11.7777777777778" customWidth="1"/>
+    <col min="19" max="19" width="11.775" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:20">
@@ -37444,7 +37516,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D156">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:D156" etc:filterBottomFollowUsedRange="0">
     <sortState ref="A1:D156">
       <sortCondition ref="C1"/>
     </sortState>
@@ -37466,32 +37538,32 @@
       <selection activeCell="AR13" sqref="AR13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.8888888888889"/>
-    <col min="2" max="2" width="17.5555555555556"/>
+    <col min="1" max="1" width="12.8916666666667"/>
+    <col min="2" max="2" width="17.5583333333333"/>
     <col min="3" max="3" width="10.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="11.8888888888889"/>
-    <col min="5" max="5" width="17.5555555555556"/>
-    <col min="6" max="6" width="11.7777777777778"/>
-    <col min="7" max="7" width="17.5555555555556"/>
-    <col min="8" max="8" width="11.7777777777778"/>
-    <col min="9" max="9" width="12.8888888888889"/>
-    <col min="10" max="10" width="13.7777777777778" style="4" customWidth="1"/>
-    <col min="11" max="11" width="11.7777777777778"/>
+    <col min="4" max="4" width="11.8916666666667"/>
+    <col min="5" max="5" width="17.5583333333333"/>
+    <col min="6" max="6" width="11.775"/>
+    <col min="7" max="7" width="17.5583333333333"/>
+    <col min="8" max="8" width="11.775"/>
+    <col min="9" max="9" width="12.8916666666667"/>
+    <col min="10" max="10" width="13.775" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.775"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="16.4444444444444"/>
+    <col min="13" max="13" width="16.4416666666667"/>
     <col min="14" max="14" width="14.3333333333333" style="10"/>
     <col min="15" max="16" width="9.66666666666667"/>
     <col min="17" max="17" width="20.6666666666667"/>
     <col min="18" max="18" width="14.3333333333333"/>
-    <col min="19" max="19" width="10.5555555555556"/>
-    <col min="20" max="20" width="12.8888888888889"/>
-    <col min="25" max="26" width="12.8888888888889"/>
+    <col min="19" max="19" width="10.5583333333333"/>
+    <col min="20" max="20" width="12.8916666666667"/>
+    <col min="25" max="26" width="12.8916666666667"/>
     <col min="27" max="27" width="9.66666666666667"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.2" spans="2:28">
+    <row r="1" ht="15" spans="2:28">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -40953,7 +41025,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D89">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:D89" etc:filterBottomFollowUsedRange="0">
     <sortState ref="A1:D89">
       <sortCondition ref="B1:B89"/>
     </sortState>
@@ -40971,11 +41043,11 @@
   <sheetPr/>
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9.66666666666667" customWidth="1"/>
     <col min="2" max="2" width="8.66666666666667" customWidth="1"/>
@@ -42437,43 +42509,67 @@
         <v>45519</v>
       </c>
       <c r="C44" s="6">
-        <v>373.1898976</v>
+        <v>392.4398953</v>
       </c>
       <c r="D44" s="8">
         <v>4</v>
       </c>
       <c r="E44" s="6">
-        <v>48.5221059736753</v>
+        <v>52.6219249781913</v>
       </c>
       <c r="F44" s="6">
-        <v>41.1028237147036</v>
+        <v>42.9566734515848</v>
       </c>
       <c r="G44" s="6">
-        <v>34.2770840364495</v>
+        <v>35.899505670253</v>
       </c>
       <c r="H44" s="6">
-        <v>32.9416132298346</v>
+        <v>34.9790055248619</v>
       </c>
       <c r="I44" s="6">
-        <v>30.7158285521431</v>
+        <v>32.6777551613841</v>
       </c>
       <c r="J44" s="6">
-        <v>35.9093261334233</v>
+        <v>38.3541727246293</v>
       </c>
       <c r="K44" s="6">
-        <v>1919.66509168635</v>
-      </c>
-    </row>
-    <row r="45" spans="3:11">
-      <c r="C45" s="6"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
+        <v>2008.07106717069</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45">
+        <v>2646</v>
+      </c>
+      <c r="B45" s="5">
+        <v>45520</v>
+      </c>
+      <c r="C45" s="6">
+        <v>385.5791327</v>
+      </c>
+      <c r="D45" s="8">
+        <v>4</v>
+      </c>
+      <c r="E45" s="6">
+        <v>68.2166539522328</v>
+      </c>
+      <c r="F45" s="6">
+        <v>35.9687811748137</v>
+      </c>
+      <c r="G45" s="6">
+        <v>36.8990082741623</v>
+      </c>
+      <c r="H45" s="6">
+        <v>26.6665101813274</v>
+      </c>
+      <c r="I45" s="6">
+        <v>37.0540461240538</v>
+      </c>
+      <c r="J45" s="6">
+        <v>30.6974942785048</v>
+      </c>
+      <c r="K45" s="6">
+        <v>2020.9183733349</v>
+      </c>
     </row>
     <row r="46" spans="3:11">
       <c r="C46" s="6"/>
@@ -42663,14 +42759,14 @@
   <sheetPr/>
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="3" width="12.8888888888889"/>
-    <col min="10" max="10" width="12.8888888888889"/>
+    <col min="3" max="3" width="12.8916666666667"/>
+    <col min="10" max="10" width="12.8916666666667"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -43551,15 +43647,25 @@
         <v>45519</v>
       </c>
       <c r="C44" s="8">
-        <v>298.133971291866</v>
+        <v>303.840039741679</v>
       </c>
       <c r="I44" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="3:9">
-      <c r="C45" s="8"/>
-      <c r="I45" s="6"/>
+    <row r="45" spans="1:9">
+      <c r="A45">
+        <v>2646</v>
+      </c>
+      <c r="B45" s="5">
+        <v>45520</v>
+      </c>
+      <c r="C45" s="8">
+        <v>297.719087635054</v>
+      </c>
+      <c r="I45" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="46" spans="3:9">
       <c r="C46" s="8"/>
@@ -43587,13 +43693,13 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="7.66666666666667" customWidth="1"/>
     <col min="2" max="2" width="5.66666666666667" customWidth="1"/>
     <col min="3" max="3" width="7.66666666666667" customWidth="1"/>
     <col min="4" max="19" width="6.66666666666667" customWidth="1"/>
-    <col min="20" max="20" width="12.8888888888889"/>
+    <col min="20" max="20" width="12.8916666666667"/>
     <col min="21" max="21" width="7.66666666666667" customWidth="1"/>
     <col min="22" max="27" width="6.66666666666667" customWidth="1"/>
   </cols>
@@ -44909,10 +45015,10 @@
       <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="5" width="12.8888888888889"/>
-    <col min="7" max="8" width="12.8888888888889"/>
+    <col min="2" max="5" width="12.8916666666667"/>
+    <col min="7" max="8" width="12.8916666666667"/>
   </cols>
   <sheetData>
     <row r="1" spans="5:8">

</xml_diff>

<commit_message>
Refactor code to improve readability and maintainability
</commit_message>
<xml_diff>
--- a/doc/绝区零下载UID.xlsx
+++ b/doc/绝区零下载UID.xlsx
@@ -14942,6 +14942,9 @@
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
                 </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -15081,6 +15084,9 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="43">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="44">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -15309,6 +15315,9 @@
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
                 </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -15443,6 +15452,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>385.5791327</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>382.9393112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15670,6 +15682,9 @@
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
                 </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -15804,6 +15819,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>68.2166539522328</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>56.8569603345142</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16031,6 +16049,9 @@
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
                 </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -16162,6 +16183,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>35.9687811748137</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>40.4145420756141</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16389,6 +16413,9 @@
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
                 </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -16517,6 +16544,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>36.8990082741623</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>32.4238341367094</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16744,6 +16774,9 @@
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
                 </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -16869,6 +16902,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>26.6665101813274</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>35.0361809628898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17095,6 +17131,9 @@
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
                 </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -17217,6 +17256,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>37.0540461240538</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>30.7334920727104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17444,6 +17486,9 @@
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
                 </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -17566,6 +17611,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>30.6974942785048</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>32.1164992159824</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17790,6 +17838,9 @@
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
                 </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -17906,6 +17957,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>2020.9183733349</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2035.47917997561</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18256,10 +18310,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>日活跃2!$B$2:$B$45</c:f>
+              <c:f>日活跃2!$B$2:$B$46</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45477</c:v>
                 </c:pt>
@@ -18391,16 +18445,19 @@
                 </c:pt>
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
+                </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>日活跃2!$C$2:$C$45</c:f>
+              <c:f>日活跃2!$C$2:$C$46</c:f>
               <c:numCache>
                 <c:formatCode>0_ </c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0">
                   <c:v>1550</c:v>
                 </c:pt>
@@ -18529,6 +18586,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>297.719087635054</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>295.627300766092</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18565,10 +18625,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>日活跃2!$B$2:$B$45</c:f>
+              <c:f>日活跃2!$B$2:$B$46</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45477</c:v>
                 </c:pt>
@@ -18700,16 +18760,19 @@
                 </c:pt>
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
+                </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>日活跃2!$D$2:$D$45</c:f>
+              <c:f>日活跃2!$D$2:$D$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="1" c:formatCode="0_ ">
                   <c:v>170</c:v>
                 </c:pt>
@@ -18793,10 +18856,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>日活跃2!$B$2:$B$45</c:f>
+              <c:f>日活跃2!$B$2:$B$46</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45477</c:v>
                 </c:pt>
@@ -18928,16 +18991,19 @@
                 </c:pt>
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
+                </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>日活跃2!$E$2:$E$45</c:f>
+              <c:f>日活跃2!$E$2:$E$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="2" c:formatCode="0_ ">
                   <c:v>100</c:v>
                 </c:pt>
@@ -19018,10 +19084,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>日活跃2!$B$2:$B$45</c:f>
+              <c:f>日活跃2!$B$2:$B$46</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45477</c:v>
                 </c:pt>
@@ -19153,16 +19219,19 @@
                 </c:pt>
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
+                </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>日活跃2!$F$2:$F$45</c:f>
+              <c:f>日活跃2!$F$2:$F$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="3" c:formatCode="0_ ">
                   <c:v>110</c:v>
                 </c:pt>
@@ -19240,10 +19309,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>日活跃2!$B$2:$B$45</c:f>
+              <c:f>日活跃2!$B$2:$B$46</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="0" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45477</c:v>
                 </c:pt>
@@ -19375,16 +19444,19 @@
                 </c:pt>
                 <c:pt idx="43" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
                   <c:v>45520</c:v>
+                </c:pt>
+                <c:pt idx="44" c:formatCode="m&quot;月&quot;d&quot;日&quot;">
+                  <c:v>45521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>日活跃2!$G$2:$G$45</c:f>
+              <c:f>日活跃2!$G$2:$G$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="44"/>
+                <c:ptCount val="45"/>
                 <c:pt idx="4" c:formatCode="0_ ">
                   <c:v>60</c:v>
                 </c:pt>
@@ -41043,8 +41115,8 @@
   <sheetPr/>
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5"/>
@@ -42571,16 +42643,40 @@
         <v>2020.9183733349</v>
       </c>
     </row>
-    <row r="46" spans="3:11">
-      <c r="C46" s="6"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
+    <row r="46" spans="1:11">
+      <c r="A46">
+        <v>2650</v>
+      </c>
+      <c r="B46" s="5">
+        <v>45521</v>
+      </c>
+      <c r="C46" s="6">
+        <v>382.9393112</v>
+      </c>
+      <c r="D46" s="8">
+        <v>4</v>
+      </c>
+      <c r="E46" s="6">
+        <v>56.8569603345142</v>
+      </c>
+      <c r="F46" s="6">
+        <v>40.4145420756141</v>
+      </c>
+      <c r="G46" s="6">
+        <v>32.4238341367094</v>
+      </c>
+      <c r="H46" s="6">
+        <v>35.0361809628898</v>
+      </c>
+      <c r="I46" s="6">
+        <v>30.7334920727104</v>
+      </c>
+      <c r="J46" s="6">
+        <v>32.1164992159824</v>
+      </c>
+      <c r="K46" s="6">
+        <v>2035.47917997561</v>
+      </c>
     </row>
     <row r="47" spans="3:11">
       <c r="C47" s="6"/>
@@ -42759,8 +42855,8 @@
   <sheetPr/>
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5"/>
@@ -43667,9 +43763,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="3:9">
-      <c r="C46" s="8"/>
-      <c r="I46" s="6"/>
+    <row r="46" spans="1:9">
+      <c r="A46">
+        <v>2650</v>
+      </c>
+      <c r="B46" s="5">
+        <v>45521</v>
+      </c>
+      <c r="C46" s="8">
+        <v>295.627300766092</v>
+      </c>
+      <c r="I46" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="47" spans="9:9">
       <c r="I47" s="6"/>

</xml_diff>